<commit_message>
added rp tasks to sprint1
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Bayne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB23B901-2661-47CC-B009-A05DB5EBCAAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5755C5-6291-4545-814F-C0EC77DE8B23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,19 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
-  <si>
-    <t>Find marriage date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare marriage date to birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="215">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -163,18 +151,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>gh(at)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(hm)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Story ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -191,411 +167,385 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Review Results</t>
+  </si>
+  <si>
+    <t>Keep doing:</t>
+  </si>
+  <si>
+    <t>Avoid:</t>
+  </si>
+  <si>
+    <t>GitHub Username</t>
+  </si>
+  <si>
+    <t>GitHub Repository:</t>
+  </si>
+  <si>
+    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
+  </si>
+  <si>
+    <t>Birth should occur before marriage of an individual</t>
+  </si>
+  <si>
+    <t>Birth should occur before death of an individual</t>
+  </si>
+  <si>
+    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
+  </si>
+  <si>
+    <t>Marriage should occur before death of either spouse</t>
+  </si>
+  <si>
+    <t>Divorce can only occur before death of both spouses</t>
+  </si>
+  <si>
+    <t>Marriage should not occur during marriage to another spouse</t>
+  </si>
+  <si>
+    <t>No more than five siblings should be born at the same time</t>
+  </si>
+  <si>
+    <t>There should be fewer than 15 siblings in a family</t>
+  </si>
+  <si>
+    <t>All male members of a family should have the same last name</t>
+  </si>
+  <si>
+    <t>Parents should not marry any of their descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry one another</t>
+  </si>
+  <si>
+    <t>First cousins should not marry one another</t>
+  </si>
+  <si>
+    <t>Aunts and uncles should not marry their nieces or nephews</t>
+  </si>
+  <si>
+    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>No more than one child with the same name and birth date should appear in a family</t>
+  </si>
+  <si>
+    <t>Include person's current age when listing individuals</t>
+  </si>
+  <si>
+    <t>List all deceased individuals in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living married people in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all multiple births in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
+  </si>
+  <si>
+    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
+  </si>
+  <si>
+    <t>Accept and use dates without days or without days and months</t>
+  </si>
+  <si>
+    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>Story Name</t>
+  </si>
+  <si>
+    <t>Story Description</t>
+  </si>
+  <si>
+    <t>Birth before death</t>
+  </si>
+  <si>
+    <t>Birth before marriage</t>
+  </si>
+  <si>
+    <t>Marriage before divorce</t>
+  </si>
+  <si>
+    <t>Marriage before death</t>
+  </si>
+  <si>
+    <t>Divorce before death</t>
+  </si>
+  <si>
+    <t>Less then 150 years old</t>
+  </si>
+  <si>
+    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
+  </si>
+  <si>
+    <t>Birth before death of parents</t>
+  </si>
+  <si>
+    <t>Child should be born before death of mother and before 9 months after death of father</t>
+  </si>
+  <si>
+    <t>Marriage after 14</t>
+  </si>
+  <si>
+    <t>No bigamy</t>
+  </si>
+  <si>
+    <t>Parents not too old</t>
+  </si>
+  <si>
+    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
+  </si>
+  <si>
+    <t>Siblings spacing</t>
+  </si>
+  <si>
+    <t>Fewer than 15 siblings</t>
+  </si>
+  <si>
+    <t>Male last names</t>
+  </si>
+  <si>
+    <t>No marriages to descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry</t>
+  </si>
+  <si>
+    <t>First cousins should not marry</t>
+  </si>
+  <si>
+    <t>Aunts and uncles</t>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+  </si>
+  <si>
+    <t>Husband in family should be male and wife in family should be female</t>
+  </si>
+  <si>
+    <t>All individual IDs should be unique and all family IDs should be unique</t>
+  </si>
+  <si>
+    <t>Unique IDs</t>
+  </si>
+  <si>
+    <t>Unique name and birth date</t>
+  </si>
+  <si>
+    <t>Unique families by spouses</t>
+  </si>
+  <si>
+    <t>Unique first names in families</t>
+  </si>
+  <si>
+    <t>Corresponding entries</t>
+  </si>
+  <si>
+    <t>Include individual ages</t>
+  </si>
+  <si>
+    <t>Order siblings by age</t>
+  </si>
+  <si>
+    <t>List deceased</t>
+  </si>
+  <si>
+    <t>List living married</t>
+  </si>
+  <si>
+    <t>List living single</t>
+  </si>
+  <si>
+    <t>List multiple births</t>
+  </si>
+  <si>
+    <t>List orphans</t>
+  </si>
+  <si>
+    <t>List recent births</t>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+  </si>
+  <si>
+    <t>List recent survivors</t>
+  </si>
+  <si>
+    <t>List upcoming birthdays</t>
+  </si>
+  <si>
+    <t>List upcoming anniversaries</t>
+  </si>
+  <si>
+    <t>Include input line numbers</t>
+  </si>
+  <si>
+    <t>List line numbers from GEDCOM source file when reporting errors</t>
+  </si>
+  <si>
+    <t>Include partial dates</t>
+  </si>
+  <si>
+    <t>Reject illegitimate dates</t>
+  </si>
+  <si>
+    <t>List large age differences</t>
+  </si>
+  <si>
+    <t>Story ID</t>
+  </si>
+  <si>
+    <t>US01</t>
+  </si>
+  <si>
+    <t>US02</t>
+  </si>
+  <si>
+    <t>US03</t>
+  </si>
+  <si>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>US06</t>
+  </si>
+  <si>
+    <t>US07</t>
+  </si>
+  <si>
+    <t>US08</t>
+  </si>
+  <si>
+    <t>US09</t>
+  </si>
+  <si>
+    <t>US10</t>
+  </si>
+  <si>
+    <t>US11</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>US13</t>
+  </si>
+  <si>
+    <t>US14</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>US28</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>US31</t>
+  </si>
+  <si>
+    <t>US32</t>
+  </si>
+  <si>
+    <t>US33</t>
+  </si>
+  <si>
+    <t>US34</t>
+  </si>
+  <si>
+    <t>US35</t>
+  </si>
+  <si>
+    <t>US36</t>
+  </si>
+  <si>
+    <t>US37</t>
+  </si>
+  <si>
+    <t>US38</t>
+  </si>
+  <si>
+    <t>US39</t>
+  </si>
+  <si>
+    <t>US40</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>US42</t>
+  </si>
+  <si>
     <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Find marriage record for individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Review Results</t>
-  </si>
-  <si>
-    <t>Keep doing:</t>
-  </si>
-  <si>
-    <t>Avoid:</t>
-  </si>
-  <si>
-    <t>GitHub Username</t>
-  </si>
-  <si>
-    <t>GitHub Repository:</t>
-  </si>
-  <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
-    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
-  </si>
-  <si>
-    <t>Birth should occur before marriage of an individual</t>
-  </si>
-  <si>
-    <t>Birth should occur before death of an individual</t>
-  </si>
-  <si>
-    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
-  </si>
-  <si>
-    <t>Marriage should occur before death of either spouse</t>
-  </si>
-  <si>
-    <t>Divorce can only occur before death of both spouses</t>
-  </si>
-  <si>
-    <t>Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
-    <t>No more than five siblings should be born at the same time</t>
-  </si>
-  <si>
-    <t>There should be fewer than 15 siblings in a family</t>
-  </si>
-  <si>
-    <t>All male members of a family should have the same last name</t>
-  </si>
-  <si>
-    <t>Parents should not marry any of their descendants</t>
-  </si>
-  <si>
-    <t>Siblings should not marry one another</t>
-  </si>
-  <si>
-    <t>First cousins should not marry one another</t>
-  </si>
-  <si>
-    <t>Aunts and uncles should not marry their nieces or nephews</t>
-  </si>
-  <si>
-    <t>No more than one individual with the same name and birth date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>No more than one child with the same name and birth date should appear in a family</t>
-  </si>
-  <si>
-    <t>Include person's current age when listing individuals</t>
-  </si>
-  <si>
-    <t>List all deceased individuals in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all living married people in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all living people over 30 who have never been married in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all multiple births in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all orphaned children (both parents dead and child &lt; 18 years old) in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>List all couples who were married when the older spouse was more than twice as old as the younger spouse</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who were born in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all living spouses and descendants of people in a GEDCOM file who died in the last 30 days</t>
-  </si>
-  <si>
-    <t>List all living people in a GEDCOM file whose birthdays occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>List all living couples in a GEDCOM file whose marriage anniversaries occur in the next 30 days</t>
-  </si>
-  <si>
-    <t>Accept and use dates without days or without days and months</t>
-  </si>
-  <si>
-    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
-  </si>
-  <si>
-    <t>Story Name</t>
-  </si>
-  <si>
-    <t>Story Description</t>
-  </si>
-  <si>
-    <t>Birth before death</t>
-  </si>
-  <si>
-    <t>Birth before marriage</t>
-  </si>
-  <si>
-    <t>Marriage before divorce</t>
-  </si>
-  <si>
-    <t>Marriage before death</t>
-  </si>
-  <si>
-    <t>Divorce before death</t>
-  </si>
-  <si>
-    <t>Less then 150 years old</t>
-  </si>
-  <si>
-    <t>Death should be less than 150 years after birth for dead people, and current date should be less than 150 years after birth for all living people</t>
-  </si>
-  <si>
-    <t>Birth before death of parents</t>
-  </si>
-  <si>
-    <t>Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
-    <t>Marriage after 14</t>
-  </si>
-  <si>
-    <t>No bigamy</t>
-  </si>
-  <si>
-    <t>Parents not too old</t>
-  </si>
-  <si>
-    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
-    <t>Siblings spacing</t>
-  </si>
-  <si>
-    <t>Fewer than 15 siblings</t>
-  </si>
-  <si>
-    <t>Male last names</t>
-  </si>
-  <si>
-    <t>No marriages to descendants</t>
-  </si>
-  <si>
-    <t>Siblings should not marry</t>
-  </si>
-  <si>
-    <t>First cousins should not marry</t>
-  </si>
-  <si>
-    <t>Aunts and uncles</t>
-  </si>
-  <si>
-    <t>Correct gender for role</t>
-  </si>
-  <si>
-    <t>Husband in family should be male and wife in family should be female</t>
-  </si>
-  <si>
-    <t>All individual IDs should be unique and all family IDs should be unique</t>
-  </si>
-  <si>
-    <t>Unique IDs</t>
-  </si>
-  <si>
-    <t>Unique name and birth date</t>
-  </si>
-  <si>
-    <t>Unique families by spouses</t>
-  </si>
-  <si>
-    <t>Unique first names in families</t>
-  </si>
-  <si>
-    <t>Corresponding entries</t>
-  </si>
-  <si>
-    <t>Include individual ages</t>
-  </si>
-  <si>
-    <t>Order siblings by age</t>
-  </si>
-  <si>
-    <t>List deceased</t>
-  </si>
-  <si>
-    <t>List living married</t>
-  </si>
-  <si>
-    <t>List living single</t>
-  </si>
-  <si>
-    <t>List multiple births</t>
-  </si>
-  <si>
-    <t>List orphans</t>
-  </si>
-  <si>
-    <t>List recent births</t>
-  </si>
-  <si>
-    <t>List recent deaths</t>
-  </si>
-  <si>
-    <t>List recent survivors</t>
-  </si>
-  <si>
-    <t>List upcoming birthdays</t>
-  </si>
-  <si>
-    <t>List upcoming anniversaries</t>
-  </si>
-  <si>
-    <t>Include input line numbers</t>
-  </si>
-  <si>
-    <t>List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
-    <t>Include partial dates</t>
-  </si>
-  <si>
-    <t>Reject illegitimate dates</t>
-  </si>
-  <si>
-    <t>List large age differences</t>
-  </si>
-  <si>
-    <t>Story ID</t>
-  </si>
-  <si>
-    <t>US01</t>
-  </si>
-  <si>
-    <t>US02</t>
-  </si>
-  <si>
-    <t>US03</t>
-  </si>
-  <si>
-    <t>US04</t>
-  </si>
-  <si>
-    <t>US05</t>
-  </si>
-  <si>
-    <t>US06</t>
-  </si>
-  <si>
-    <t>US07</t>
-  </si>
-  <si>
-    <t>US08</t>
-  </si>
-  <si>
-    <t>US09</t>
-  </si>
-  <si>
-    <t>US10</t>
-  </si>
-  <si>
-    <t>US11</t>
-  </si>
-  <si>
-    <t>US12</t>
-  </si>
-  <si>
-    <t>US13</t>
-  </si>
-  <si>
-    <t>US14</t>
-  </si>
-  <si>
-    <t>US15</t>
-  </si>
-  <si>
-    <t>US16</t>
-  </si>
-  <si>
-    <t>US17</t>
-  </si>
-  <si>
-    <t>US18</t>
-  </si>
-  <si>
-    <t>US19</t>
-  </si>
-  <si>
-    <t>US20</t>
-  </si>
-  <si>
-    <t>US21</t>
-  </si>
-  <si>
-    <t>US22</t>
-  </si>
-  <si>
-    <t>US23</t>
-  </si>
-  <si>
-    <t>US24</t>
-  </si>
-  <si>
-    <t>US25</t>
-  </si>
-  <si>
-    <t>US26</t>
-  </si>
-  <si>
-    <t>US27</t>
-  </si>
-  <si>
-    <t>US28</t>
-  </si>
-  <si>
-    <t>US29</t>
-  </si>
-  <si>
-    <t>US30</t>
-  </si>
-  <si>
-    <t>US31</t>
-  </si>
-  <si>
-    <t>US32</t>
-  </si>
-  <si>
-    <t>US33</t>
-  </si>
-  <si>
-    <t>US34</t>
-  </si>
-  <si>
-    <t>US35</t>
-  </si>
-  <si>
-    <t>US36</t>
-  </si>
-  <si>
-    <t>US37</t>
-  </si>
-  <si>
-    <t>US38</t>
-  </si>
-  <si>
-    <t>US39</t>
-  </si>
-  <si>
-    <t>US40</t>
-  </si>
-  <si>
-    <t>US41</t>
-  </si>
-  <si>
-    <t>US42</t>
-  </si>
-  <si>
-    <t>T05.01</t>
-  </si>
-  <si>
-    <t>T05.02</t>
-  </si>
-  <si>
-    <t>T05.03</t>
-  </si>
-  <si>
-    <t>Coding</t>
   </si>
   <si>
     <t>Dates before current date</t>
@@ -718,9 +668,6 @@
     <t>List married</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>T22.01</t>
   </si>
   <si>
@@ -730,13 +677,49 @@
     <t>T22.02</t>
   </si>
   <si>
-    <t>Check if ID exists in HashMap</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
     <t>mattbayne</t>
+  </si>
+  <si>
+    <t>Check if ID exists as key in HashMap</t>
+  </si>
+  <si>
+    <t>T01.01</t>
+  </si>
+  <si>
+    <t>Convert GEDCOM date argument into java.util.Date object</t>
+  </si>
+  <si>
+    <t>T01.02</t>
+  </si>
+  <si>
+    <t>Check if date is before today's date</t>
+  </si>
+  <si>
+    <t>T42.01</t>
+  </si>
+  <si>
+    <t>T42.02</t>
+  </si>
+  <si>
+    <t>Try to convert GEDCOM date argument into java.util.Date object</t>
+  </si>
+  <si>
+    <t>Check if conversion fails or not</t>
+  </si>
+  <si>
+    <t>Communicating frequently</t>
+  </si>
+  <si>
+    <t>Not committing code to github often</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>esavova</t>
   </si>
 </sst>
 </file>
@@ -747,7 +730,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -776,6 +759,17 @@
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -869,7 +863,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -897,6 +891,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1146,10 +1142,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>42796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1162,9 +1155,6 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,102 +2044,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2174,177 +2167,183 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1875" customWidth="1"/>
-    <col min="2" max="2" width="7.6171875" customWidth="1"/>
-    <col min="3" max="3" width="25.6171875" customWidth="1"/>
-    <col min="4" max="4" width="6.6171875" customWidth="1"/>
-    <col min="5" max="5" width="10.1875" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+    <sortCondition ref="B2:B10"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2359,72 +2358,72 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="7"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.37890625" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2438,9 +2437,9 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2463,9 +2462,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2488,9 +2487,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2513,9 +2512,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2547,73 +2546,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="2"/>
-    <col min="2" max="2" width="16.6171875" customWidth="1"/>
-    <col min="3" max="3" width="12.47265625" customWidth="1"/>
-    <col min="4" max="4" width="7.1875" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>40442</v>
+        <v>42796</v>
       </c>
       <c r="B2">
         <v>36</v>
       </c>
       <c r="D2">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
-        <v>40455</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <f>B2-B3</f>
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>250</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
-      </c>
-      <c r="F3" s="9">
-        <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2626,248 +2603,297 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6171875" customWidth="1"/>
-    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6171875" customWidth="1"/>
-    <col min="5" max="5" width="8.37890625" customWidth="1"/>
-    <col min="6" max="6" width="9.5234375" customWidth="1"/>
-    <col min="7" max="7" width="8.47265625" customWidth="1"/>
-    <col min="8" max="8" width="7.6171875" customWidth="1"/>
-    <col min="9" max="9" width="10.80859375" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-      <c r="I2" s="6">
-        <v>42794</v>
       </c>
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" s="7"/>
       <c r="K3" s="1"/>
-      <c r="R3" s="6"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" t="s">
-        <v>193</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I4" s="7"/>
       <c r="K4" s="1"/>
-      <c r="R4" s="6"/>
-    </row>
-    <row r="5" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C5" t="s">
-        <v>193</v>
-      </c>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="7"/>
       <c r="K5" s="1"/>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7">
+        <v>179</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="K7" s="1"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="K8" s="1"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="7"/>
+      <c r="K9" s="1"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="K11" s="1"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K13" s="1"/>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="F14">
         <v>20</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E8">
+      <c r="K14" s="1"/>
+      <c r="R14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="F15">
         <v>20</v>
       </c>
-      <c r="J8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K15" s="1"/>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K16" s="1"/>
+      <c r="R16" s="6"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K17" s="1"/>
+      <c r="R17" s="6"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K18" s="1"/>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K19" s="1"/>
+      <c r="R19" s="6"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8">
-        <v>200</v>
-      </c>
-      <c r="O8">
-        <v>120</v>
-      </c>
-      <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="K9" s="1"/>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" spans="1:18" ht="49.2" x14ac:dyDescent="0.4">
-      <c r="J10" t="s">
-        <v>167</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
-      <c r="J11" t="s">
-        <v>168</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" ht="49.2" x14ac:dyDescent="0.4">
-      <c r="J12" t="s">
-        <v>169</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B14" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="B21" s="1" t="s">
-        <v>44</v>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2885,35 +2911,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2931,35 +2957,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2976,35 +3002,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3015,493 +3041,520 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="C12" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C15" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="12" t="s">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="12" t="s">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="12" t="s">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="12" t="s">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="12" t="s">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="12" t="s">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="12" t="s">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="D31" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="12" t="s">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="12" t="s">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="12" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="12" t="s">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="12" t="s">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="12" t="s">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="12" t="s">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>150</v>
-      </c>
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C41" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="D41" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="12" t="s">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>157</v>
-      </c>
-      <c r="B34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>159</v>
-      </c>
-      <c r="B36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>162</v>
-      </c>
-      <c r="B39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>165</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>76</v>
+      <c r="D43" s="17" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more stories to backlog
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjayathrey/Downloads/CS-555-Project-Group-7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Bayne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66733FE8-52C4-1444-BDFE-2C556C2385D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2715ED-437E-4FF3-84B8-FBB70773A291}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="216">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1005,7 +1005,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1076,7 +1076,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2047,18 +2047,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2170,22 +2170,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2344,6 +2344,86 @@
       </c>
       <c r="E10" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2364,47 +2444,47 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2427,7 +2507,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2443,7 +2523,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2468,7 +2548,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2493,7 +2573,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2518,7 +2598,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2558,17 +2638,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.80859375" style="2"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.47265625" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>42796</v>
       </c>
@@ -2615,19 +2695,19 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2678,7 +2758,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -2692,7 +2772,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -2703,12 +2783,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -2730,7 +2810,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -2744,7 +2824,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -2758,12 +2838,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2785,7 +2865,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -2796,7 +2876,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -2809,11 +2889,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -2835,7 +2915,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -2857,47 +2937,47 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.4">
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.4">
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.4">
       <c r="K19" s="1"/>
       <c r="R19" s="6"/>
     </row>
-    <row r="21" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
         <v>212</v>
       </c>
@@ -2917,9 +2997,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2963,9 +3043,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3008,9 +3088,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3049,17 +3129,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3073,7 +3153,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3087,7 +3167,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3098,7 +3178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3109,7 +3189,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3120,7 +3200,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3131,7 +3211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3142,7 +3222,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3153,7 +3233,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3164,7 +3244,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3175,7 +3255,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3189,7 +3269,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3200,7 +3280,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3211,7 +3291,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3222,7 +3302,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3233,7 +3313,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3244,7 +3324,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3255,7 +3335,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3266,7 +3346,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3277,7 +3357,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3288,7 +3368,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3299,7 +3379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3310,7 +3390,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3321,7 +3401,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3332,7 +3412,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3343,7 +3423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3354,7 +3434,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3368,7 +3448,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3382,7 +3462,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3393,7 +3473,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3407,7 +3487,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3421,7 +3501,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3432,7 +3512,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3443,7 +3523,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3454,7 +3534,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3465,7 +3545,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3476,7 +3556,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3487,7 +3567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3498,7 +3578,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3509,7 +3589,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3520,7 +3600,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3534,7 +3614,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3545,7 +3625,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated burndown sheet, backlog and sprint one
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D603EC24-8B60-48BA-9F38-6A4C50A0D69E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7B47D0-AD6E-4FB9-B636-50964A79CF42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="219">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -726,6 +726,12 @@
   </si>
   <si>
     <t>Marriage After 14</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1143,24 +1149,30 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42796</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>42810</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,13 +1703,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>948267</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>160867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>397934</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
@@ -2175,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2219,7 +2231,7 @@
         <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2250,7 +2262,7 @@
         <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2329,7 +2341,7 @@
         <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2736,51 +2748,93 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="2">
         <v>42796</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>36</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42810</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3" s="9">
+        <f>E3/F3</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2795,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2851,13 +2905,22 @@
         <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="F2">
         <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
@@ -2882,6 +2945,9 @@
       </c>
       <c r="B4" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>179</v>
       </c>
       <c r="I4" s="7"/>
       <c r="K4" s="1"/>
@@ -2903,13 +2969,22 @@
         <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E6">
         <v>25</v>
       </c>
       <c r="F6">
         <v>30</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
@@ -2958,13 +3033,22 @@
         <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E10">
         <v>25</v>
       </c>
       <c r="F10">
         <v>30</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
@@ -2975,6 +3059,9 @@
       </c>
       <c r="B11" s="1" t="s">
         <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>179</v>
       </c>
       <c r="I11" s="7"/>
       <c r="K11" s="1"/>
@@ -3310,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
claimed 2 stories for sprint 2
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Bayne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7B47D0-AD6E-4FB9-B636-50964A79CF42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FA328-AF1F-439E-B795-3C94B0BDB2AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="219">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2066,14 +2066,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2187,20 +2187,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.1875" customWidth="1"/>
+    <col min="2" max="2" width="7.6171875" customWidth="1"/>
+    <col min="3" max="3" width="25.6171875" customWidth="1"/>
+    <col min="4" max="4" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="10.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>153</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>117</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>118</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>119</v>
       </c>
@@ -2404,15 +2404,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2</v>
+      </c>
       <c r="B16" t="s">
         <v>120</v>
       </c>
       <c r="C16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>121</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>122</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -2436,7 +2442,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>134</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>128</v>
       </c>
@@ -2453,15 +2459,21 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>2</v>
+      </c>
       <c r="B22" t="s">
         <v>125</v>
       </c>
       <c r="C22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>129</v>
       </c>
@@ -2470,7 +2482,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>131</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>134</v>
       </c>
@@ -2486,7 +2498,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>138</v>
       </c>
@@ -2494,7 +2506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>141</v>
       </c>
@@ -2502,7 +2514,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>144</v>
       </c>
@@ -2510,7 +2522,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>148</v>
       </c>
@@ -2518,7 +2530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>149</v>
       </c>
@@ -2526,7 +2538,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>151</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>152</v>
       </c>
@@ -2560,47 +2572,47 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2623,7 +2635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2639,7 +2651,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2689,7 +2701,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2754,17 +2766,17 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" style="2"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.80859375" style="2"/>
+    <col min="3" max="3" width="16.6171875" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" customWidth="1"/>
+    <col min="5" max="5" width="7.1875" customWidth="1"/>
+    <col min="6" max="6" width="6.80859375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -2801,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2822,17 +2834,17 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2853,19 +2865,19 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="1" max="1" width="7.6171875" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="8.37890625" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
+    <col min="8" max="8" width="7.6171875" customWidth="1"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2894,7 +2906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2925,7 +2937,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -2939,7 +2951,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -2953,12 +2965,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -2989,7 +3001,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3003,7 +3015,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3017,12 +3029,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3053,7 +3065,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3067,7 +3079,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3080,11 +3092,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3106,7 +3118,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3128,7 +3140,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -3147,7 +3159,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -3166,7 +3178,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3185,7 +3197,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -3204,7 +3216,7 @@
       <c r="K19" s="1"/>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -3221,31 +3233,31 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
         <v>212</v>
       </c>
@@ -3265,9 +3277,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3311,9 +3323,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3356,9 +3368,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3401,13 +3413,13 @@
       <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3421,7 +3433,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3435,7 +3447,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3446,7 +3458,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3457,7 +3469,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3468,7 +3480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3479,7 +3491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3490,7 +3502,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3501,7 +3513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3512,7 +3524,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3523,7 +3535,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3537,7 +3549,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3548,7 +3560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3559,7 +3571,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3570,7 +3582,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3581,7 +3593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3592,7 +3604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3603,7 +3615,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3614,7 +3626,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3625,7 +3637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3636,7 +3648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3658,7 +3670,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3669,7 +3681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3680,7 +3692,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3691,7 +3703,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3702,7 +3714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3716,7 +3728,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3730,7 +3742,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3755,7 +3767,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3769,7 +3781,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3780,7 +3792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3791,7 +3803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3802,7 +3814,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3813,7 +3825,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3824,7 +3836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3835,7 +3847,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3846,7 +3858,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3857,7 +3869,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3868,7 +3880,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3882,7 +3894,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3893,7 +3905,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
completed sprint1 and filled in sprint2
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjayathrey/Downloads/CS-555-Project-Group-7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Bayne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA842F0C-707E-BF44-A6E0-D314EC96BBBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9642773-31B6-4324-B19F-77F2C6A9005D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="12560" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="7275" windowWidth="29040" windowHeight="15225" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="226">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1035,7 +1035,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1106,7 +1106,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2087,14 +2087,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2209,19 +2209,19 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2331,10 +2331,10 @@
         <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2348,10 +2348,10 @@
         <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>153</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>118</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>119</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2450,8 +2450,11 @@
       <c r="D16" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>121</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>122</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>134</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>128</v>
       </c>
@@ -2492,7 +2495,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2505,8 +2508,11 @@
       <c r="D22" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="E22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>129</v>
       </c>
@@ -2515,7 +2521,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>131</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>134</v>
       </c>
@@ -2531,7 +2537,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>138</v>
       </c>
@@ -2539,7 +2545,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>141</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>144</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>148</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>149</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>151</v>
       </c>
@@ -2579,7 +2585,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>152</v>
       </c>
@@ -2605,47 +2611,47 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2684,7 +2690,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2734,7 +2740,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2799,17 +2805,17 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10.80859375" style="2"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.80859375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2867,17 +2873,17 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2895,22 +2901,22 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2970,7 +2976,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -2984,7 +2990,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -2998,12 +3004,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3034,7 +3040,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3048,7 +3054,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3062,12 +3068,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3098,7 +3104,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3112,7 +3118,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3125,11 +3131,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>187</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E14">
         <v>15</v>
@@ -3148,10 +3154,19 @@
       <c r="F14">
         <v>20</v>
       </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>218</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3162,7 +3177,7 @@
         <v>187</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -3170,10 +3185,19 @@
       <c r="F15">
         <v>20</v>
       </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>218</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3204,7 +3228,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="56" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3214,7 +3238,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3245,7 +3269,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3256,7 +3280,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3273,7 +3297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3290,31 +3314,31 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
@@ -3328,15 +3352,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="21.80859375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3363,6 +3390,46 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3380,9 +3447,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3425,9 +3492,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3466,17 +3533,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:B39"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3490,7 +3557,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3504,7 +3571,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3515,7 +3582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3526,7 +3593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3537,7 +3604,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3548,7 +3615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3559,7 +3626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3570,7 +3637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3581,7 +3648,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3592,7 +3659,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3606,7 +3673,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3617,7 +3684,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3628,7 +3695,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3639,7 +3706,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3650,7 +3717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3661,7 +3728,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3672,7 +3739,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3683,7 +3750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3694,7 +3761,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3705,7 +3772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3716,7 +3783,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3727,7 +3794,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3738,7 +3805,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3749,7 +3816,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3760,7 +3827,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3771,7 +3838,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3785,7 +3852,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3799,7 +3866,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3810,7 +3877,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3824,7 +3891,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3838,7 +3905,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3849,7 +3916,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3860,7 +3927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3871,7 +3938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3882,7 +3949,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3893,7 +3960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3904,7 +3971,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3915,7 +3982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3926,7 +3993,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3937,7 +4004,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3951,7 +4018,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3962,7 +4029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated for sprint 2
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Bayne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9642773-31B6-4324-B19F-77F2C6A9005D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45293D8-22EC-4F06-9EC0-C0DDE8E105C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7275" windowWidth="29040" windowHeight="15225" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="226">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -819,12 +819,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -896,7 +905,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -926,6 +935,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2083,18 +2095,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2111,7 +2123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2145,7 +2157,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2162,7 +2174,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2179,7 +2191,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2206,22 +2218,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2238,7 +2250,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2255,7 +2267,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2268,8 +2280,11 @@
       <c r="D3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2286,7 +2301,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2299,8 +2314,11 @@
       <c r="D5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2317,7 +2335,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2334,7 +2352,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2351,7 +2369,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2368,151 +2386,181 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <v>1</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>190</v>
       </c>
-      <c r="E11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+        <v>187</v>
+      </c>
+      <c r="E13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="19">
+        <v>2</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>121</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>122</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>134</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>187</v>
-      </c>
-      <c r="E22" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>129</v>
       </c>
@@ -2521,7 +2569,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>131</v>
       </c>
@@ -2529,73 +2577,57 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
-        <v>151</v>
-      </c>
-      <c r="C31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
-    <sortCondition ref="B2:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+    <sortCondition ref="A2:A30"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2608,50 +2640,50 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="7"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2674,7 +2706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2690,7 +2722,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2715,7 +2747,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2740,7 +2772,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2765,7 +2797,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2802,20 +2834,20 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.80859375" style="2"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.47265625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.80859375" customWidth="1"/>
-    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -2838,7 +2870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -2852,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2873,17 +2905,17 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2901,22 +2933,22 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G14" sqref="G14:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.47265625" customWidth="1"/>
-    <col min="7" max="7" width="8.47265625" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.80859375" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2945,7 +2977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2976,7 +3008,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -2990,7 +3022,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3004,12 +3036,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3040,7 +3072,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3054,7 +3086,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3068,12 +3100,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3104,7 +3136,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3118,7 +3150,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3131,11 +3163,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3166,7 +3198,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3197,7 +3229,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3228,7 +3260,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3238,7 +3270,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3269,7 +3301,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3280,7 +3312,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3297,7 +3329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3314,31 +3346,31 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
@@ -3352,18 +3384,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.80859375" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3392,7 +3424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3412,7 +3444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3430,6 +3462,102 @@
       </c>
       <c r="F3">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3447,9 +3575,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3492,9 +3620,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3533,17 +3661,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3557,7 +3685,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3571,7 +3699,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3582,7 +3710,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3593,7 +3721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3604,7 +3732,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3615,7 +3743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3626,7 +3754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3637,7 +3765,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3648,7 +3776,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3659,7 +3787,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3673,7 +3801,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3684,7 +3812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3695,7 +3823,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3706,7 +3834,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3717,7 +3845,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3728,7 +3856,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3739,7 +3867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3750,7 +3878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3761,7 +3889,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3772,7 +3900,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3783,7 +3911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3794,7 +3922,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3805,7 +3933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3816,7 +3944,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3827,7 +3955,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3838,7 +3966,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3852,7 +3980,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3866,7 +3994,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3877,7 +4005,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3891,7 +4019,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3905,7 +4033,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3916,7 +4044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3927,7 +4055,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3938,7 +4066,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3949,7 +4077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3960,7 +4088,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3971,7 +4099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3982,7 +4110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3993,7 +4121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4004,7 +4132,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4018,7 +4146,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4029,7 +4157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
added sprint 1 review list
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45293D8-22EC-4F06-9EC0-C0DDE8E105C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B7C214-E5A3-40F6-89FF-C3916ACF76BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="228">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -753,6 +753,12 @@
   </si>
   <si>
     <t>Compare using birth date and potential death date using after() in java.util.Date</t>
+  </si>
+  <si>
+    <t>Not pulling from Github enough</t>
+  </si>
+  <si>
+    <t>Giving feedback to other team members</t>
   </si>
 </sst>
 </file>
@@ -2095,7 +2101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2930,10 +2936,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3365,6 +3371,11 @@
         <v>211</v>
       </c>
     </row>
+    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
@@ -3373,6 +3384,11 @@
     <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated report/added us28 test cases
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C985B3-9728-45B2-9473-37DE85497618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC9D09E-3334-47B9-BD2D-908310C25A91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="234">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -759,6 +759,24 @@
   </si>
   <si>
     <t>Giving feedback to other team members</t>
+  </si>
+  <si>
+    <t>T28.01</t>
+  </si>
+  <si>
+    <t>T28.02</t>
+  </si>
+  <si>
+    <t>Parse file to get all siblings</t>
+  </si>
+  <si>
+    <t>Get age of all siblings</t>
+  </si>
+  <si>
+    <t>T28.03</t>
+  </si>
+  <si>
+    <t>For each family sort siblings</t>
   </si>
 </sst>
 </file>
@@ -911,7 +929,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -944,6 +962,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1198,6 +1219,9 @@
                 <c:pt idx="1">
                   <c:v>42810</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>42824</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1212,6 +1236,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,7 +2128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2227,7 +2254,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2530,7 +2557,7 @@
         <v>179</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2840,7 +2867,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2905,9 +2932,11 @@
         <v>8</v>
       </c>
       <c r="E3">
+        <f>SUM(Sprint1!G2:G21)</f>
         <v>229</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
+        <f>SUM(Sprint1!H2:H21)</f>
         <v>190</v>
       </c>
       <c r="G3" s="9">
@@ -2918,6 +2947,28 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>165</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42824</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D6" si="0">C3-C4</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>SUM(Sprint2!G2:G21)</f>
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>SUM(Sprint2!H2:H21)</f>
+        <v>30</v>
+      </c>
+      <c r="G4" s="9">
+        <f>E4/F4</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2942,7 +2993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -3428,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3619,13 +3670,73 @@
         <v>179</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
         <v>20</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented US05 and US06
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Desktop\CS 555 Software Dev\Group Project\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC9D09E-3334-47B9-BD2D-908310C25A91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F2C4E0-7F08-4586-B55E-2EE8EDE0FE24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="249">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -777,6 +777,51 @@
   </si>
   <si>
     <t>For each family sort siblings</t>
+  </si>
+  <si>
+    <t>T05.01</t>
+  </si>
+  <si>
+    <t>Check Family for marriage tag</t>
+  </si>
+  <si>
+    <t>Check if Marriage date exists</t>
+  </si>
+  <si>
+    <t>For both spouces check if death exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For both spouces check if marriage is before death </t>
+  </si>
+  <si>
+    <t>T05.02</t>
+  </si>
+  <si>
+    <t>T05.03</t>
+  </si>
+  <si>
+    <t>T05.04</t>
+  </si>
+  <si>
+    <t>T06.01</t>
+  </si>
+  <si>
+    <t>T06.02</t>
+  </si>
+  <si>
+    <t>T06.03</t>
+  </si>
+  <si>
+    <t>T06.04</t>
+  </si>
+  <si>
+    <t>Check Family for divorce tag</t>
+  </si>
+  <si>
+    <t>Check if divorce date exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For both spouces check if divorce is before death </t>
   </si>
 </sst>
 </file>
@@ -929,7 +974,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -963,6 +1008,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2128,18 +2176,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2156,7 +2204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2173,7 +2221,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2190,7 +2238,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2207,7 +2255,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2224,7 +2272,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2257,16 +2305,16 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.1875" customWidth="1"/>
+    <col min="2" max="2" width="7.6171875" customWidth="1"/>
+    <col min="3" max="3" width="25.6171875" customWidth="1"/>
+    <col min="4" max="4" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="10.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2283,7 +2331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2300,7 +2348,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2317,7 +2365,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2334,7 +2382,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2351,7 +2399,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2368,7 +2416,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2385,7 +2433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2402,7 +2450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2419,7 +2467,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2436,7 +2484,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2450,7 +2498,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2464,7 +2512,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2481,7 +2529,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2498,7 +2546,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2515,7 +2563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2529,7 +2577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2543,7 +2591,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2560,7 +2608,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>121</v>
       </c>
@@ -2568,7 +2616,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>122</v>
       </c>
@@ -2576,7 +2624,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -2584,7 +2632,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>128</v>
       </c>
@@ -2593,7 +2641,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>129</v>
       </c>
@@ -2602,7 +2650,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>131</v>
       </c>
@@ -2610,7 +2658,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>138</v>
       </c>
@@ -2618,7 +2666,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>144</v>
       </c>
@@ -2626,7 +2674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>148</v>
       </c>
@@ -2634,7 +2682,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>149</v>
       </c>
@@ -2642,7 +2690,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>151</v>
       </c>
@@ -2650,7 +2698,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>152</v>
       </c>
@@ -2676,47 +2724,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2739,7 +2787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2755,7 +2803,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2780,7 +2828,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2805,7 +2853,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2830,7 +2878,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2870,17 +2918,17 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" style="2"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.80859375" style="2"/>
+    <col min="3" max="3" width="16.6171875" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" customWidth="1"/>
+    <col min="5" max="5" width="7.1875" customWidth="1"/>
+    <col min="6" max="6" width="6.80859375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -2903,7 +2951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -2917,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2944,7 +2992,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -2955,7 +3003,7 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D6" si="0">C3-C4</f>
+        <f t="shared" ref="D4" si="0">C3-C4</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -2971,12 +3019,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2997,19 +3045,19 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="1" max="1" width="7.6171875" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="8.37890625" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
+    <col min="8" max="8" width="7.6171875" customWidth="1"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3038,7 +3086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3069,7 +3117,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3083,7 +3131,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3097,12 +3145,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3133,7 +3181,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3147,7 +3195,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3161,12 +3209,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3197,7 +3245,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3211,7 +3259,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3224,11 +3272,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3259,7 +3307,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3290,7 +3338,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3321,7 +3369,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3331,7 +3379,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3362,7 +3410,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3373,7 +3421,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3402,7 +3450,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3431,41 +3479,41 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
         <v>226</v>
       </c>
@@ -3479,18 +3527,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3519,7 +3567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3539,7 +3587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3559,7 +3607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3579,7 +3627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3599,7 +3647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>153</v>
       </c>
@@ -3619,7 +3667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -3639,12 +3687,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>119</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="23" t="s">
+        <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
         <v>180</v>
@@ -3652,90 +3700,199 @@
       <c r="D8" t="s">
         <v>156</v>
       </c>
-      <c r="E8">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="F12">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B17" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C17" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="E9">
+      <c r="E17">
         <v>20</v>
       </c>
-      <c r="F9">
+      <c r="F17">
         <v>20</v>
       </c>
-      <c r="G9">
+      <c r="G17">
         <v>15</v>
       </c>
-      <c r="H9">
+      <c r="H17">
         <v>30</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B18" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C18" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I18" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B19" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C19" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D19" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I19" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C20" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I20" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3754,9 +3911,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3799,9 +3956,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3840,17 +3997,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3864,7 +4021,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3878,7 +4035,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3889,7 +4046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3900,7 +4057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3911,7 +4068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3922,7 +4079,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3933,7 +4090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3944,7 +4101,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3955,7 +4112,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3966,7 +4123,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3980,7 +4137,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3991,7 +4148,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4002,7 +4159,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4013,7 +4170,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4024,7 +4181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4035,7 +4192,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4046,7 +4203,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4057,7 +4214,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4068,7 +4225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4079,7 +4236,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4090,7 +4247,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4101,7 +4258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4112,7 +4269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4123,7 +4280,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4134,7 +4291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4145,7 +4302,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4159,7 +4316,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4173,7 +4330,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4184,7 +4341,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4198,7 +4355,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4212,7 +4369,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4223,7 +4380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4234,7 +4391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4245,7 +4402,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4256,7 +4413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4267,7 +4424,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4278,7 +4435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4289,7 +4446,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4300,7 +4457,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4311,7 +4468,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4325,7 +4482,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4336,7 +4493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
added some user stories to backlog
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5406F3C-616C-4CAC-96E0-C218F6ACB126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58411FFF-69AC-433F-A89A-F92D88FA2AF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="253">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2311,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2374,7 +2374,7 @@
         <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2408,7 +2408,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2627,106 +2627,142 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="12"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>129</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" t="s">
-        <v>85</v>
-      </c>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>152</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
-    <sortCondition ref="A2:A30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:E31">
+    <sortCondition descending="1" ref="A19:A31"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2932,7 +2968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -4067,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added sprint 3 user stories for rp
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58411FFF-69AC-433F-A89A-F92D88FA2AF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D228F95-19BF-421A-B081-854197312D9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="253">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2313,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4011,13 +4011,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -4046,6 +4049,40 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in burndown for sprint 1
Remaining stories for sprint 1 in the burndown sheet said 28 when it wswas actually 27
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D228F95-19BF-421A-B081-854197312D9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E78CE0-6E95-4B69-AD51-E97DC9039854}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1295,10 +1295,10 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2968,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3027,11 +3027,11 @@
         <v>42810</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <f>C2-C3</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <f>SUM(Sprint1!G2:G21)</f>
@@ -3054,7 +3054,7 @@
         <v>42824</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4" si="0">C3-C4</f>
@@ -4013,7 +4013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4022,7 +4022,7 @@
     <col min="2" max="2" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Excel Document is not Completely complete
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92b94c44c6b04b3e/Spring 2021/CS555/PROJECT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Desktop\CS 555 Software Dev\Group Project\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{12A6E7A8-A64C-0543-8CB9-E61C93EF38F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{612D8A5F-FFB4-49F2-9261-CF9A6D4D4585}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7933F657-19EB-474B-AFB0-73B6CCBFE1F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7275" windowWidth="29040" windowHeight="15225" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -852,6 +852,18 @@
   </si>
   <si>
     <t>Check husband/wife if marriage occurs before their birth</t>
+  </si>
+  <si>
+    <t>Altering other people's code without warning.</t>
+  </si>
+  <si>
+    <t>Not notifying when we make changes.</t>
+  </si>
+  <si>
+    <t>Re-using old helper functions.</t>
+  </si>
+  <si>
+    <t>Letting each other know when we are pushing to GitHub.</t>
   </si>
 </sst>
 </file>
@@ -2209,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -2335,7 +2347,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -2738,19 +2750,31 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>3</v>
+      </c>
       <c r="B25" t="s">
         <v>131</v>
       </c>
       <c r="C25" t="s">
         <v>85</v>
       </c>
+      <c r="D25" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>3</v>
+      </c>
       <c r="B26" t="s">
         <v>136</v>
       </c>
       <c r="C26" t="s">
         <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
@@ -3017,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3144,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -3630,10 +3654,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4119,6 +4143,47 @@
         <v>221</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B28" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B31" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B32" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B34" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B35" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B36" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4128,10 +4193,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4268,6 +4333,40 @@
       </c>
       <c r="F7">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4325,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4736,7 +4835,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
updated table with US31
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Desktop\CS 555 Software Dev\Group Project\CS-555-Project-Group-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7933F657-19EB-474B-AFB0-73B6CCBFE1F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2315D6-0914-4E9C-B693-E79AB0A96A01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1315,6 +1315,9 @@
                 <c:pt idx="2">
                   <c:v>42824</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>42838</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1332,6 +1335,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,18 +2227,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2249,7 +2255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2346,20 +2352,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2376,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2427,7 +2433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2648,7 +2654,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2678,8 +2684,11 @@
       <c r="D19" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E19" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2692,8 +2701,11 @@
       <c r="D20" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2707,7 +2719,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2721,7 +2733,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2735,7 +2747,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2749,7 +2761,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2763,21 +2775,22 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="19">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="19" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>138</v>
       </c>
@@ -2785,7 +2798,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>146</v>
       </c>
@@ -2793,7 +2806,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>147</v>
       </c>
@@ -2801,7 +2814,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>148</v>
       </c>
@@ -2809,7 +2822,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>149</v>
       </c>
@@ -2817,7 +2830,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>151</v>
       </c>
@@ -2825,7 +2838,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>152</v>
       </c>
@@ -2851,47 +2864,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="7"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2914,7 +2927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2930,7 +2943,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2955,7 +2968,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2980,7 +2993,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -3005,7 +3018,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -3042,20 +3055,20 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.80859375" style="2"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.47265625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.80859375" customWidth="1"/>
-    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -3078,7 +3091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -3092,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -3119,7 +3132,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -3130,7 +3143,7 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4" si="0">C3-C4</f>
+        <f t="shared" ref="D4:D5" si="0">C3-C4</f>
         <v>8</v>
       </c>
       <c r="E4">
@@ -3146,12 +3159,34 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B5" s="2">
+        <v>42838</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>SUM(Sprint3!G2:G40)</f>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f>SUM(Sprint3!H2:H40)</f>
+        <v>5</v>
+      </c>
+      <c r="G5" s="9">
+        <f>E5/F5</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -3172,19 +3207,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.47265625" customWidth="1"/>
-    <col min="7" max="7" width="8.47265625" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.80859375" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3213,7 +3248,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3244,7 +3279,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3258,7 +3293,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3272,12 +3307,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3308,7 +3343,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3322,7 +3357,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3336,12 +3371,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3372,7 +3407,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3386,7 +3421,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3399,11 +3434,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3434,7 +3469,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3465,7 +3500,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3496,7 +3531,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3506,7 +3541,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3537,7 +3572,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3548,7 +3583,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3577,7 +3612,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3606,41 +3641,41 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>226</v>
       </c>
@@ -3660,12 +3695,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3694,7 +3729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3723,7 +3758,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3752,7 +3787,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3781,7 +3816,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>256</v>
       </c>
@@ -3789,7 +3824,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>257</v>
       </c>
@@ -3797,7 +3832,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3826,7 +3861,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>253</v>
       </c>
@@ -3834,7 +3869,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>254</v>
       </c>
@@ -3842,7 +3877,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3871,7 +3906,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>249</v>
       </c>
@@ -3885,7 +3920,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>250</v>
       </c>
@@ -3899,7 +3934,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3928,7 +3963,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>234</v>
       </c>
@@ -3942,7 +3977,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>239</v>
       </c>
@@ -3956,7 +3991,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>240</v>
       </c>
@@ -3970,7 +4005,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>241</v>
       </c>
@@ -3984,7 +4019,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4010,7 +4045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>242</v>
       </c>
@@ -4024,7 +4059,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>243</v>
       </c>
@@ -4038,7 +4073,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>244</v>
       </c>
@@ -4052,7 +4087,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>245</v>
       </c>
@@ -4063,7 +4098,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4092,7 +4127,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>228</v>
       </c>
@@ -4109,7 +4144,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>229</v>
       </c>
@@ -4126,7 +4161,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>232</v>
       </c>
@@ -4143,43 +4178,43 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>259</v>
       </c>
@@ -4195,16 +4230,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4233,7 +4268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4250,7 +4285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4266,8 +4301,17 @@
       <c r="F3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -4284,7 +4328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4301,7 +4345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4318,7 +4362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4335,7 +4379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4352,7 +4396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4383,9 +4427,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4428,13 +4472,13 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4448,7 +4492,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4462,7 +4506,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4473,7 +4517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4484,7 +4528,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4495,7 +4539,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4509,7 +4553,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4523,7 +4567,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4534,7 +4578,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4545,7 +4589,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4556,7 +4600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4570,7 +4614,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4581,7 +4625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4592,7 +4636,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4603,7 +4647,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4614,7 +4658,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4625,7 +4669,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4636,7 +4680,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4647,7 +4691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4658,7 +4702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4669,7 +4713,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4680,7 +4724,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4691,7 +4735,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4702,7 +4746,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4713,7 +4757,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4724,7 +4768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4735,7 +4779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4749,7 +4793,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4763,7 +4807,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4774,7 +4818,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4788,7 +4832,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4802,7 +4846,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4813,7 +4857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4824,7 +4868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4835,7 +4879,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4846,7 +4890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4857,7 +4901,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4868,7 +4912,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4879,7 +4923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4890,7 +4934,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4901,7 +4945,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4915,7 +4959,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4926,7 +4970,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated report for US21
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25434009-F712-43E3-BF5F-A712A1448508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703255FF-A5AD-4AB1-97AE-19ED76D4B020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1337,7 +1337,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2352,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2685,7 +2685,7 @@
         <v>179</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3054,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3167,23 +3167,23 @@
         <v>42838</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <f>SUM(Sprint3!G2:G40)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <f>SUM(Sprint3!H2:H40)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G5" s="9">
         <f>E5/F5</f>
-        <v>1.8</v>
+        <v>1.2666666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4230,13 +4230,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -4326,6 +4326,15 @@
       </c>
       <c r="F4">
         <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
completed all sprint 3 sheet info
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92b94c44c6b04b3e/Spring 2021/CS555/PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703255FF-A5AD-4AB1-97AE-19ED76D4B020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{703255FF-A5AD-4AB1-97AE-19ED76D4B020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BCF12F7C-2FBC-499D-BF65-8705796180FB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12456" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2231,14 +2231,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2352,20 +2352,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.1875" customWidth="1"/>
+    <col min="2" max="2" width="7.6171875" customWidth="1"/>
+    <col min="3" max="3" width="25.6171875" customWidth="1"/>
+    <col min="4" max="4" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="10.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2746,8 +2746,11 @@
       <c r="D23" s="24" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2760,8 +2763,11 @@
       <c r="D24" s="24" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2790,7 +2796,7 @@
       </c>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>138</v>
       </c>
@@ -2798,7 +2804,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>146</v>
       </c>
@@ -2806,7 +2812,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>147</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>148</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>149</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>151</v>
       </c>
@@ -2838,7 +2844,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>152</v>
       </c>
@@ -2864,47 +2870,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2943,7 +2949,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -3054,21 +3060,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" style="2"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.80859375" style="2"/>
+    <col min="3" max="3" width="16.6171875" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" customWidth="1"/>
+    <col min="5" max="5" width="7.1875" customWidth="1"/>
+    <col min="6" max="6" width="6.80859375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -3159,7 +3165,7 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -3174,19 +3180,17 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f>SUM(Sprint3!G2:G40)</f>
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="F5">
-        <f>SUM(Sprint3!H2:H40)</f>
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="G5" s="9">
         <f>E5/F5</f>
-        <v>1.2666666666666666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.1176470588235294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -3207,19 +3211,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="1" max="1" width="7.6171875" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="8.37890625" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
+    <col min="8" max="8" width="7.6171875" customWidth="1"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3248,7 +3252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3279,7 +3283,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3293,7 +3297,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3307,12 +3311,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3343,7 +3347,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3357,7 +3361,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3371,12 +3375,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="7.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3407,7 +3411,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3421,7 +3425,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3434,11 +3438,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3469,7 +3473,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3500,7 +3504,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3531,7 +3535,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3541,7 +3545,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3572,7 +3576,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3583,7 +3587,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3612,7 +3616,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3641,41 +3645,41 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
         <v>226</v>
       </c>
@@ -3695,12 +3699,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="37.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3729,7 +3733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3787,7 +3791,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3816,7 +3820,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="23" t="s">
         <v>256</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="23" t="s">
         <v>257</v>
       </c>
@@ -3832,7 +3836,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3861,7 +3865,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="23" t="s">
         <v>253</v>
       </c>
@@ -3869,7 +3873,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="23" t="s">
         <v>254</v>
       </c>
@@ -3877,7 +3881,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3906,7 +3910,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="23" t="s">
         <v>249</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="23" t="s">
         <v>250</v>
       </c>
@@ -3934,7 +3938,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3963,7 +3967,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="23" t="s">
         <v>234</v>
       </c>
@@ -3977,7 +3981,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="23" t="s">
         <v>239</v>
       </c>
@@ -3991,7 +3995,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="23" t="s">
         <v>240</v>
       </c>
@@ -4005,7 +4009,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="23" t="s">
         <v>241</v>
       </c>
@@ -4019,7 +4023,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4045,7 +4049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
         <v>242</v>
       </c>
@@ -4059,7 +4063,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="23" t="s">
         <v>243</v>
       </c>
@@ -4073,7 +4077,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="23" t="s">
         <v>244</v>
       </c>
@@ -4087,7 +4091,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="23" t="s">
         <v>245</v>
       </c>
@@ -4098,7 +4102,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4127,7 +4131,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="22" t="s">
         <v>228</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="22" t="s">
         <v>229</v>
       </c>
@@ -4161,7 +4165,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="22" t="s">
         <v>232</v>
       </c>
@@ -4178,43 +4182,43 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>259</v>
       </c>
@@ -4231,15 +4235,15 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.37890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4268,7 +4272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4285,7 +4289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4311,7 +4315,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -4337,7 +4341,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4354,7 +4358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4370,8 +4374,17 @@
       <c r="F6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4387,8 +4400,17 @@
       <c r="F7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4405,7 +4427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4436,9 +4458,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4477,17 +4499,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4501,7 +4523,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4515,7 +4537,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4526,7 +4548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4537,7 +4559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4548,7 +4570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4562,7 +4584,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4576,7 +4598,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4586,8 +4608,11 @@
       <c r="C8" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4598,7 +4623,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4609,7 +4634,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4623,7 +4648,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4634,7 +4659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4644,8 +4669,11 @@
       <c r="C13" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4656,7 +4684,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4667,7 +4695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4677,8 +4705,11 @@
       <c r="C16" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4688,8 +4719,11 @@
       <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4700,7 +4734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4711,7 +4745,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4722,7 +4756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4733,7 +4767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4744,7 +4778,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4755,7 +4789,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4766,7 +4800,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4777,7 +4811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4788,7 +4822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4802,7 +4836,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4816,7 +4850,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4827,7 +4861,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4841,7 +4875,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4855,7 +4889,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4866,7 +4900,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4877,7 +4911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4888,7 +4922,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4899,7 +4933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4910,7 +4944,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4921,7 +4955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4932,7 +4966,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4943,7 +4977,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4954,7 +4988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4968,7 +5002,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4979,7 +5013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated for sprint 4 rp
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjayathrey/Downloads/CS-555-Project-Group-7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7276D2D-9B3F-5646-BD94-B6FDEBC534B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D981BF-94C4-4DAD-A2BA-976846157BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23140" windowHeight="12460" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="263">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1167,7 +1167,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1238,7 +1238,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2231,14 +2231,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2352,20 +2352,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D28" sqref="B27:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2812,8 +2812,11 @@
       <c r="C27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D27" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>4</v>
       </c>
@@ -2823,8 +2826,11 @@
       <c r="C28" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D28" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>4</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2849,7 +2855,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2903,47 +2909,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2982,7 +2988,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -3007,7 +3013,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -3097,17 +3103,17 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -3171,7 +3177,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>1.1176470588235294</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -3244,19 +3250,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3316,7 +3322,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3330,7 +3336,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -3344,12 +3350,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3380,7 +3386,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -3394,7 +3400,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -3408,12 +3414,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3444,7 +3450,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -3458,7 +3464,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -3471,11 +3477,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3506,7 +3512,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3537,7 +3543,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3568,7 +3574,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="56" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -3578,7 +3584,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3609,7 +3615,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -3620,7 +3626,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3649,7 +3655,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3678,41 +3684,41 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>226</v>
       </c>
@@ -3732,12 +3738,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3795,7 +3801,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3824,7 +3830,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>256</v>
       </c>
@@ -3861,7 +3867,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>257</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>253</v>
       </c>
@@ -3906,7 +3912,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>254</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3943,7 +3949,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>249</v>
       </c>
@@ -3957,7 +3963,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>250</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -4000,7 +4006,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>234</v>
       </c>
@@ -4014,7 +4020,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>239</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>240</v>
       </c>
@@ -4042,7 +4048,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>241</v>
       </c>
@@ -4056,7 +4062,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4082,7 +4088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>242</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>243</v>
       </c>
@@ -4110,7 +4116,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>244</v>
       </c>
@@ -4124,7 +4130,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>245</v>
       </c>
@@ -4135,7 +4141,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4164,7 +4170,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>228</v>
       </c>
@@ -4181,7 +4187,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>229</v>
       </c>
@@ -4198,7 +4204,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>232</v>
       </c>
@@ -4215,43 +4221,43 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>259</v>
       </c>
@@ -4271,12 +4277,12 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4305,7 +4311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -4374,7 +4380,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4400,7 +4406,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4426,7 +4432,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4469,7 +4475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4494,15 +4500,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4531,7 +4540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4548,7 +4557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4563,6 +4572,40 @@
       </c>
       <c r="F3">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4575,17 +4618,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4599,7 +4642,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4613,7 +4656,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4624,7 +4667,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4635,7 +4678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4646,7 +4689,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4660,7 +4703,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4674,7 +4717,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4688,7 +4731,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4702,7 +4745,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4716,7 +4759,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4730,7 +4773,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4741,7 +4784,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4755,7 +4798,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4766,7 +4809,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4777,7 +4820,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4791,7 +4834,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4805,7 +4848,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4816,7 +4859,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4827,7 +4870,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4838,7 +4881,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4849,7 +4892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4860,7 +4903,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4871,7 +4914,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4882,7 +4925,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4893,7 +4936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4904,7 +4947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4918,7 +4961,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4932,7 +4975,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4943,7 +4986,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4957,7 +5000,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4971,7 +5014,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4982,7 +5025,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4993,7 +5036,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5004,7 +5047,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5015,7 +5058,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5029,7 +5072,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5043,7 +5086,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5054,7 +5097,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5065,7 +5108,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5076,7 +5119,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5090,7 +5133,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5101,7 +5144,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Completed Sprint 3 code part
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Desktop\CS 555 Software Dev\Group Project\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D981BF-94C4-4DAD-A2BA-976846157BB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74858D6E-61FE-43AF-A749-FECE22CB7604}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="262">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -543,9 +543,6 @@
   </si>
   <si>
     <t>US42</t>
-  </si>
-  <si>
-    <t>Coding</t>
   </si>
   <si>
     <t>Dates before current date</t>
@@ -1337,7 +1334,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2231,14 +2228,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2255,80 +2252,80 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>179</v>
       </c>
-      <c r="B3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2352,20 +2349,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="B27:D28"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.1875" customWidth="1"/>
+    <col min="2" max="2" width="7.6171875" customWidth="1"/>
+    <col min="3" max="3" width="25.6171875" customWidth="1"/>
+    <col min="4" max="4" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="10.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2379,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2390,16 +2387,16 @@
         <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2410,13 +2407,13 @@
         <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2427,13 +2424,13 @@
         <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2441,16 +2438,16 @@
         <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2461,13 +2458,13 @@
         <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2478,13 +2475,13 @@
         <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2492,16 +2489,16 @@
         <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2512,13 +2509,13 @@
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2529,13 +2526,13 @@
         <v>68</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2546,13 +2543,13 @@
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2563,13 +2560,13 @@
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2580,13 +2577,13 @@
         <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2597,13 +2594,13 @@
         <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2614,13 +2611,13 @@
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2631,13 +2628,13 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2648,13 +2645,13 @@
         <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2665,13 +2662,13 @@
         <v>97</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2682,13 +2679,13 @@
         <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2699,13 +2696,13 @@
         <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2713,16 +2710,16 @@
         <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2733,13 +2730,13 @@
         <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2750,13 +2747,13 @@
         <v>82</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2767,13 +2764,13 @@
         <v>83</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E24" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2784,10 +2781,13 @@
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2798,11 +2798,13 @@
         <v>92</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2813,10 +2815,10 @@
         <v>94</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="21">
         <v>4</v>
       </c>
@@ -2827,10 +2829,10 @@
         <v>102</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="21">
         <v>4</v>
       </c>
@@ -2841,7 +2843,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2852,10 +2854,10 @@
         <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2866,10 +2868,10 @@
         <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2879,8 +2881,11 @@
       <c r="C32" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2889,6 +2894,9 @@
       </c>
       <c r="C33" t="s">
         <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2909,49 +2917,49 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="7"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2972,9 +2980,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2988,9 +2996,9 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -3013,9 +3021,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -3038,9 +3046,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -3063,9 +3071,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -3100,22 +3108,22 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" style="2"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.80859375" style="2"/>
+    <col min="3" max="3" width="16.6171875" customWidth="1"/>
+    <col min="4" max="4" width="12.47265625" customWidth="1"/>
+    <col min="5" max="5" width="7.1875" customWidth="1"/>
+    <col min="6" max="6" width="6.80859375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -3136,9 +3144,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2">
         <v>42796</v>
@@ -3150,9 +3158,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2">
         <v>42810</v>
@@ -3177,9 +3185,9 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="2">
         <v>42824</v>
@@ -3204,19 +3212,19 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="2">
         <v>42838</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>95</v>
@@ -3229,9 +3237,9 @@
         <v>1.1176470588235294</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3250,19 +3258,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="1" max="1" width="7.6171875" customWidth="1"/>
+    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6171875" customWidth="1"/>
+    <col min="5" max="5" width="8.37890625" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
+    <col min="8" max="8" width="7.6171875" customWidth="1"/>
+    <col min="9" max="9" width="10.80859375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3282,16 +3290,16 @@
         <v>14</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3299,10 +3307,10 @@
         <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -3317,56 +3325,56 @@
         <v>5</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I3" s="7"/>
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I4" s="7"/>
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -3381,45 +3389,45 @@
         <v>15</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="7"/>
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I8" s="7"/>
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3427,10 +3435,10 @@
         <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10">
         <v>25</v>
@@ -3445,43 +3453,43 @@
         <v>20</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I11" s="7"/>
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3489,10 +3497,10 @@
         <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E14">
         <v>15</v>
@@ -3507,12 +3515,12 @@
         <v>20</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3520,10 +3528,10 @@
         <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -3538,12 +3546,12 @@
         <v>20</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3551,10 +3559,10 @@
         <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -3569,22 +3577,22 @@
         <v>15</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3592,10 +3600,10 @@
         <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18">
         <v>30</v>
@@ -3610,34 +3618,34 @@
         <v>20</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>123</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E20">
         <v>40</v>
@@ -3652,21 +3660,21 @@
         <v>20</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>139</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E21">
         <v>75</v>
@@ -3681,46 +3689,46 @@
         <v>55</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3738,12 +3746,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="37.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3772,7 +3780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3780,10 +3788,10 @@
         <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -3798,10 +3806,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3809,10 +3817,10 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -3827,10 +3835,10 @@
         <v>30</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3838,10 +3846,10 @@
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -3856,26 +3864,26 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="B5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="B6" t="s">
         <v>257</v>
       </c>
-      <c r="B6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3883,10 +3891,10 @@
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -3901,26 +3909,26 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="B8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="B9" t="s">
         <v>254</v>
       </c>
-      <c r="B9" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3928,10 +3936,10 @@
         <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -3946,38 +3954,38 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>251</v>
       </c>
-      <c r="C11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" t="s">
-        <v>252</v>
-      </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3985,10 +3993,10 @@
         <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -4003,66 +4011,66 @@
         <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" t="s">
         <v>234</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" t="s">
         <v>235</v>
       </c>
-      <c r="C14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>236</v>
       </c>
-      <c r="C15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>237</v>
       </c>
-      <c r="C16" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="B17" t="s">
-        <v>238</v>
-      </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4070,10 +4078,10 @@
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18">
         <v>10</v>
@@ -4088,60 +4096,60 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>246</v>
       </c>
-      <c r="C19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+      <c r="C20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B22" t="s">
         <v>247</v>
       </c>
-      <c r="C20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" t="s">
-        <v>237</v>
-      </c>
-      <c r="C21" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22" t="s">
-        <v>248</v>
-      </c>
       <c r="D22" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4149,10 +4157,10 @@
         <v>97</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E23">
         <v>20</v>
@@ -4167,99 +4175,99 @@
         <v>30</v>
       </c>
       <c r="I23" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="I24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B25" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="I24" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="C25" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="I25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="I25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>233</v>
-      </c>
       <c r="C26" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I26" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -4274,15 +4282,15 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.37890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4311,7 +4319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4319,7 +4327,7 @@
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -4328,7 +4336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4336,7 +4344,7 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -4351,18 +4359,18 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -4377,10 +4385,10 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4388,7 +4396,7 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -4403,10 +4411,10 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4414,7 +4422,7 @@
         <v>82</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -4429,10 +4437,10 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4440,7 +4448,7 @@
         <v>83</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -4455,10 +4463,10 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4466,7 +4474,7 @@
         <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -4474,8 +4482,17 @@
       <c r="F8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4483,13 +4500,22 @@
         <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9">
         <v>10</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4500,18 +4526,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23.6171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4540,7 +4566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4548,7 +4574,7 @@
         <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -4557,7 +4583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4565,7 +4591,7 @@
         <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -4574,7 +4600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -4582,7 +4608,7 @@
         <v>94</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -4591,7 +4617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -4599,12 +4625,46 @@
         <v>102</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
       <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
         <v>10</v>
       </c>
     </row>
@@ -4618,17 +4678,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4639,24 +4699,24 @@
         <v>67</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4667,7 +4727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4678,7 +4738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4689,7 +4749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4700,10 +4760,10 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4714,10 +4774,10 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4728,24 +4788,24 @@
         <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4756,10 +4816,10 @@
         <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4767,13 +4827,13 @@
         <v>77</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4784,7 +4844,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4795,10 +4855,10 @@
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4806,21 +4866,21 @@
         <v>81</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4831,10 +4891,10 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4845,10 +4905,10 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4859,7 +4919,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4869,8 +4929,11 @@
       <c r="C19" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4881,7 +4944,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4892,7 +4955,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4903,7 +4966,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4914,7 +4977,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4924,8 +4987,11 @@
       <c r="C24" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4936,7 +5002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4947,7 +5013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4955,13 +5021,13 @@
         <v>95</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4972,10 +5038,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4983,10 +5049,10 @@
         <v>97</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4997,10 +5063,10 @@
         <v>53</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5011,10 +5077,10 @@
         <v>54</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5025,7 +5091,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5036,7 +5102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5047,7 +5113,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5058,7 +5124,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5069,10 +5135,10 @@
         <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5083,10 +5149,10 @@
         <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5097,7 +5163,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5107,8 +5173,11 @@
       <c r="C39" s="12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5118,8 +5187,11 @@
       <c r="C40" s="12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5130,10 +5202,10 @@
         <v>109</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5144,7 +5216,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -5155,7 +5227,7 @@
         <v>65</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
report ready for sprint 3 submission
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellie\Desktop\CS 555 Software Dev\Group Project\CS-555-Project-Group-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74858D6E-61FE-43AF-A749-FECE22CB7604}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A30D920-2BAE-4173-A994-0CD0D11FCEA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="265">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -861,6 +861,15 @@
   </si>
   <si>
     <t>Letting each other know when we are pushing to GitHub.</t>
+  </si>
+  <si>
+    <t>Get work done ahead of time so there is time for integration testing</t>
+  </si>
+  <si>
+    <t>Lack of communication</t>
+  </si>
+  <si>
+    <t>Push regularly</t>
   </si>
 </sst>
 </file>
@@ -2224,18 +2233,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2252,7 +2261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2269,7 +2278,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2320,7 +2329,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2350,19 +2359,19 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C33"/>
+      <selection activeCell="A29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1875" customWidth="1"/>
-    <col min="2" max="2" width="7.6171875" customWidth="1"/>
-    <col min="3" max="3" width="25.6171875" customWidth="1"/>
-    <col min="4" max="4" width="6.6171875" customWidth="1"/>
-    <col min="5" max="5" width="10.1875" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2379,7 +2388,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2396,7 +2405,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2464,7 +2473,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2498,7 +2507,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2532,7 +2541,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2617,7 +2626,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2634,7 +2643,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2651,7 +2660,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2668,7 +2677,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2685,7 +2694,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2702,7 +2711,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2719,7 +2728,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2736,7 +2745,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2753,7 +2762,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2770,7 +2779,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>4</v>
       </c>
@@ -2832,7 +2841,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>4</v>
       </c>
@@ -2842,8 +2851,11 @@
       <c r="C29" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D29" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2857,7 +2869,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2871,7 +2883,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2885,7 +2897,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2917,47 +2929,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="7"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.37890625" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2996,7 +3008,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3021,7 +3033,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3046,7 +3058,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3108,20 +3120,20 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.80859375" style="2"/>
-    <col min="3" max="3" width="16.6171875" customWidth="1"/>
-    <col min="4" max="4" width="12.47265625" customWidth="1"/>
-    <col min="5" max="5" width="7.1875" customWidth="1"/>
-    <col min="6" max="6" width="6.80859375" customWidth="1"/>
-    <col min="7" max="7" width="12.47265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>161</v>
       </c>
@@ -3144,7 +3156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -3185,7 +3197,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3212,7 +3224,7 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3227,17 +3239,19 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <v>95</v>
-      </c>
-      <c r="F5">
-        <v>85</v>
+        <f>SUM(Sprint3!G2:G27)</f>
+        <v>212</v>
+      </c>
+      <c r="F5" s="9">
+        <f>SUM(Sprint3!H2:H27)</f>
+        <v>100</v>
       </c>
       <c r="G5" s="9">
         <f>E5/F5</f>
-        <v>1.1176470588235294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -3258,19 +3272,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6171875" customWidth="1"/>
-    <col min="2" max="2" width="24.47265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6171875" customWidth="1"/>
-    <col min="5" max="5" width="8.37890625" customWidth="1"/>
-    <col min="6" max="6" width="9.47265625" customWidth="1"/>
-    <col min="7" max="7" width="8.47265625" customWidth="1"/>
-    <col min="8" max="8" width="7.6171875" customWidth="1"/>
-    <col min="9" max="9" width="10.80859375" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3299,7 +3313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3330,7 +3344,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -3344,7 +3358,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -3358,12 +3372,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3394,7 +3408,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -3408,7 +3422,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>204</v>
       </c>
@@ -3422,12 +3436,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3458,7 +3472,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -3472,7 +3486,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -3485,11 +3499,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3520,7 +3534,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3551,7 +3565,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3582,7 +3596,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>222</v>
       </c>
@@ -3592,7 +3606,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3623,7 +3637,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="36.9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>223</v>
       </c>
@@ -3634,7 +3648,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3663,7 +3677,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3692,41 +3706,41 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>225</v>
       </c>
@@ -3743,15 +3757,15 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B28" sqref="B28:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.1875" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3780,7 +3794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3809,7 +3823,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3838,7 +3852,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3867,7 +3881,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>255</v>
       </c>
@@ -3875,7 +3889,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>256</v>
       </c>
@@ -3883,7 +3897,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3912,7 +3926,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>252</v>
       </c>
@@ -3920,7 +3934,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>253</v>
       </c>
@@ -3928,7 +3942,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3957,7 +3971,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>248</v>
       </c>
@@ -3971,7 +3985,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>249</v>
       </c>
@@ -3985,7 +3999,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -4014,7 +4028,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>233</v>
       </c>
@@ -4028,7 +4042,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>238</v>
       </c>
@@ -4042,7 +4056,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>239</v>
       </c>
@@ -4056,7 +4070,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>240</v>
       </c>
@@ -4070,7 +4084,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4096,7 +4110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>241</v>
       </c>
@@ -4110,7 +4124,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>242</v>
       </c>
@@ -4124,7 +4138,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>243</v>
       </c>
@@ -4138,7 +4152,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>244</v>
       </c>
@@ -4149,7 +4163,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4178,7 +4192,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>227</v>
       </c>
@@ -4195,7 +4209,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>228</v>
       </c>
@@ -4212,7 +4226,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>231</v>
       </c>
@@ -4229,43 +4243,43 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>258</v>
       </c>
@@ -4279,18 +4293,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.37890625" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4319,7 +4333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4329,14 +4343,26 @@
       <c r="C2" t="s">
         <v>178</v>
       </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4346,6 +4372,9 @@
       <c r="C3" t="s">
         <v>178</v>
       </c>
+      <c r="D3" t="s">
+        <v>216</v>
+      </c>
       <c r="E3">
         <v>5</v>
       </c>
@@ -4362,7 +4391,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -4372,6 +4401,9 @@
       <c r="C4" t="s">
         <v>189</v>
       </c>
+      <c r="D4" t="s">
+        <v>216</v>
+      </c>
       <c r="E4">
         <v>10</v>
       </c>
@@ -4388,7 +4420,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4398,6 +4430,9 @@
       <c r="C5" t="s">
         <v>189</v>
       </c>
+      <c r="D5" t="s">
+        <v>216</v>
+      </c>
       <c r="E5">
         <v>10</v>
       </c>
@@ -4414,7 +4449,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4424,6 +4459,9 @@
       <c r="C6" s="24" t="s">
         <v>186</v>
       </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
       <c r="E6">
         <v>10</v>
       </c>
@@ -4440,7 +4478,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4450,6 +4488,9 @@
       <c r="C7" s="24" t="s">
         <v>186</v>
       </c>
+      <c r="D7" t="s">
+        <v>216</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
@@ -4466,7 +4507,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4476,6 +4517,9 @@
       <c r="C8" t="s">
         <v>179</v>
       </c>
+      <c r="D8" t="s">
+        <v>216</v>
+      </c>
       <c r="E8">
         <v>15</v>
       </c>
@@ -4492,7 +4536,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4502,6 +4546,9 @@
       <c r="C9" t="s">
         <v>179</v>
       </c>
+      <c r="D9" t="s">
+        <v>216</v>
+      </c>
       <c r="E9">
         <v>10</v>
       </c>
@@ -4516,6 +4563,45 @@
       </c>
       <c r="I9" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4526,18 +4612,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.6171875" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4566,7 +4652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4583,7 +4669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4600,7 +4686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -4617,7 +4703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -4634,7 +4720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -4651,7 +4737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -4666,6 +4752,23 @@
       </c>
       <c r="F7">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4678,17 +4781,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.47265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4702,7 +4805,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4716,7 +4819,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4727,7 +4830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4738,7 +4841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4749,7 +4852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4763,7 +4866,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4777,7 +4880,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4791,7 +4894,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4805,7 +4908,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4819,7 +4922,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4833,7 +4936,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4844,7 +4947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4858,7 +4961,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4869,7 +4972,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4880,7 +4983,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4894,7 +4997,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4908,7 +5011,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4919,7 +5022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4933,7 +5036,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4944,7 +5047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4955,7 +5058,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4966,7 +5069,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4977,7 +5080,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4991,7 +5094,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -5002,7 +5105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -5013,7 +5116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -5027,7 +5130,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -5041,7 +5144,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -5052,7 +5155,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -5066,7 +5169,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5080,7 +5183,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5091,7 +5194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5102,7 +5205,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5113,7 +5216,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5124,7 +5227,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5138,7 +5241,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5152,7 +5255,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5163,7 +5266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5177,7 +5280,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5191,7 +5294,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5205,7 +5308,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5216,7 +5319,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated Team report for sprint 4 and added review comments
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjayathrey/Downloads/CS-555-Project-Group-7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanp\Documents\Stevens\Spring 2021\Agile Methods for Soft. Dev\CS-555-Project-Group-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAA3AA1-E173-5849-AF74-DBD0E980C868}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046828AC-4AFE-4C21-943A-1D815D6A86CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="268">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -867,6 +867,15 @@
   </si>
   <si>
     <t>Push regularly</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Strong finish done ahead of time</t>
+  </si>
+  <si>
+    <t>Being careless when dealing with merge conflicts</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1034,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1073,6 +1082,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="66" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="66" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="66"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="66" applyFill="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1183,7 +1193,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1254,7 +1264,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2253,14 +2263,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2277,7 +2287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2294,7 +2304,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2311,7 +2321,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2328,7 +2338,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2345,7 +2355,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2374,20 +2384,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2404,7 +2414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2421,7 +2431,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2438,7 +2448,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2455,7 +2465,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2472,7 +2482,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2489,7 +2499,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2506,7 +2516,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -2557,7 +2567,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2574,7 +2584,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2591,7 +2601,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2625,7 +2635,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2642,7 +2652,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2659,7 +2669,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2676,7 +2686,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -2693,7 +2703,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2710,7 +2720,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2727,7 +2737,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2744,7 +2754,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2761,7 +2771,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2778,7 +2788,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2795,7 +2805,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2812,7 +2822,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2829,7 +2839,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2846,7 +2856,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>4</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>4</v>
       </c>
@@ -2876,9 +2886,11 @@
       <c r="D29" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="E29" s="25"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E29" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2895,7 +2907,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2912,7 +2924,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2929,7 +2941,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2964,47 +2976,47 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3027,7 +3039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3043,7 +3055,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3068,7 +3080,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3093,7 +3105,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3118,7 +3130,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3155,20 +3167,20 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>161</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -3232,7 +3244,7 @@
         <v>1.2052631578947368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3243,7 +3255,7 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">C3-C4</f>
+        <f t="shared" ref="D4:D6" si="0">C3-C4</f>
         <v>8</v>
       </c>
       <c r="E4">
@@ -3259,7 +3271,7 @@
         <v>1.0661764705882353</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3286,7 +3298,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -3296,17 +3308,21 @@
       <c r="C6" s="27">
         <v>0</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E6" s="27">
-        <v>67</v>
+        <f>SUM(Sprint4!G2:G8)</f>
+        <v>132</v>
       </c>
       <c r="F6" s="29">
-        <v>40</v>
-      </c>
-      <c r="G6" s="29">
-        <v>0.92500000000000004</v>
+        <f>SUM(Sprint4!H2:H8)</f>
+        <v>110</v>
+      </c>
+      <c r="G6" s="9">
+        <f>E6/F6</f>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -3325,19 +3341,19 @@
       <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3366,7 +3382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -3397,7 +3413,7 @@
       <c r="K2" s="1"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -3411,7 +3427,7 @@
       <c r="K3" s="1"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -3425,12 +3441,12 @@
       <c r="K4" s="1"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3461,7 +3477,7 @@
       <c r="K6" s="1"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -3475,7 +3491,7 @@
       <c r="K7" s="1"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>204</v>
       </c>
@@ -3489,12 +3505,12 @@
       <c r="K8" s="1"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="7.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
       <c r="K9" s="1"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -3525,7 +3541,7 @@
       <c r="K10" s="1"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -3539,7 +3555,7 @@
       <c r="K11" s="1"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -3552,11 +3568,11 @@
       <c r="K12" s="1"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K13" s="1"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="19.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3587,7 +3603,7 @@
       <c r="K14" s="1"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3618,7 +3634,7 @@
       <c r="K15" s="1"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3649,7 +3665,7 @@
       <c r="K16" s="1"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="56" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>222</v>
       </c>
@@ -3659,7 +3675,7 @@
       <c r="K17" s="1"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3690,7 +3706,7 @@
       <c r="K18" s="1"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>223</v>
       </c>
@@ -3701,7 +3717,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3730,7 +3746,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -3759,41 +3775,41 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>225</v>
       </c>
@@ -3813,12 +3829,12 @@
       <selection activeCell="B28" sqref="B28:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3847,7 +3863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3876,7 +3892,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3905,7 +3921,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3934,7 +3950,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>255</v>
       </c>
@@ -3942,7 +3958,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>256</v>
       </c>
@@ -3950,7 +3966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3979,7 +3995,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>252</v>
       </c>
@@ -3987,7 +4003,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>253</v>
       </c>
@@ -3995,7 +4011,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -4024,7 +4040,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>248</v>
       </c>
@@ -4038,7 +4054,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>249</v>
       </c>
@@ -4052,7 +4068,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -4081,7 +4097,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>233</v>
       </c>
@@ -4095,7 +4111,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>238</v>
       </c>
@@ -4109,7 +4125,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>239</v>
       </c>
@@ -4123,7 +4139,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>240</v>
       </c>
@@ -4137,7 +4153,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -4163,7 +4179,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>241</v>
       </c>
@@ -4177,7 +4193,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>242</v>
       </c>
@@ -4191,7 +4207,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>243</v>
       </c>
@@ -4205,7 +4221,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>244</v>
       </c>
@@ -4216,7 +4232,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>141</v>
       </c>
@@ -4245,7 +4261,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>227</v>
       </c>
@@ -4262,7 +4278,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>228</v>
       </c>
@@ -4279,7 +4295,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>231</v>
       </c>
@@ -4296,43 +4312,43 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>258</v>
       </c>
@@ -4349,15 +4365,15 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B12" sqref="B12:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4386,7 +4402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4415,7 +4431,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4444,7 +4460,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -4473,7 +4489,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -4502,7 +4518,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4531,7 +4547,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4560,7 +4576,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4589,7 +4605,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -4618,41 +4634,41 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>264</v>
       </c>
@@ -4665,18 +4681,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4705,7 +4721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4731,7 +4747,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4757,7 +4773,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -4773,8 +4789,17 @@
       <c r="F4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -4790,8 +4815,17 @@
       <c r="F5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -4817,7 +4851,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -4843,7 +4877,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -4859,6 +4893,52 @@
       <c r="F8">
         <v>15</v>
       </c>
+      <c r="G8" s="31">
+        <v>25</v>
+      </c>
+      <c r="H8" s="31">
+        <v>20</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4874,13 +4954,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4894,7 +4974,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4908,7 +4988,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4919,7 +4999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4930,7 +5010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4941,7 +5021,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4955,7 +5035,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4969,7 +5049,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4983,7 +5063,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4997,7 +5077,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -5011,7 +5091,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -5025,7 +5105,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -5036,7 +5116,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -5050,7 +5130,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -5061,7 +5141,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -5072,7 +5152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -5086,7 +5166,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -5100,7 +5180,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -5111,7 +5191,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -5125,7 +5205,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -5136,7 +5216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -5147,7 +5227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -5158,7 +5238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -5169,7 +5249,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -5183,7 +5263,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -5194,7 +5274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -5205,7 +5285,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -5219,7 +5299,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -5233,7 +5313,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -5244,7 +5324,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -5258,7 +5338,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5272,7 +5352,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5283,7 +5363,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5294,7 +5374,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5305,7 +5385,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5316,7 +5396,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5330,7 +5410,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5344,7 +5424,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5355,7 +5435,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5369,7 +5449,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5383,7 +5463,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5397,7 +5477,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5408,7 +5488,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>